<commit_message>
se agrego nueva linea
</commit_message>
<xml_diff>
--- a/objetivos.xlsx
+++ b/objetivos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bladimir\Documents\UCC\Semestre 9\Arquitectura de Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bladimir\Documents\UCC\Semestre 9\Arquitectura de Software\Documentos Arquitectura\ArquitecturaDeSoftware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFDB159-3B7F-4299-8024-524E70F62108}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956F19D9-FB64-476A-A76A-A4C60B669FD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F1EFE7E0-B9EB-44F4-B156-3B1D7406B858}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Objetivo 1</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Monitorear los signos vitales de los pacientes a traves de un software con alarmas de situaciones adversas o fuera de los limites deseados, con transmision de informacion al gobierno a traves de una base datos blockchain público</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
 </sst>
 </file>
@@ -301,6 +304,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -315,9 +321,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7892F872-D04B-4CD1-9288-946739352F24}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,55 +673,55 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -730,15 +733,15 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
@@ -748,7 +751,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -766,7 +769,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="12"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
@@ -778,7 +781,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="9"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
@@ -811,13 +814,13 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C10"/>
@@ -825,6 +828,11 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
se agrego trabajo final
</commit_message>
<xml_diff>
--- a/objetivos.xlsx
+++ b/objetivos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bladimir\Documents\UCC\Semestre 9\Arquitectura de Software\Documentos Arquitectura\ArquitecturaDeSoftware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FBC32A-05B5-4298-9B20-66E6D4277221}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A796A40D-237D-4224-B734-9987FF97EBB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F1EFE7E0-B9EB-44F4-B156-3B1D7406B858}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F1EFE7E0-B9EB-44F4-B156-3B1D7406B858}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos" sheetId="1" r:id="rId1"/>
@@ -287,26 +287,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -321,6 +306,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7892F872-D04B-4CD1-9288-946739352F24}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -665,7 +666,7 @@
       <c r="B2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
@@ -673,55 +674,55 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="8"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -733,15 +734,15 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
@@ -751,7 +752,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -769,7 +770,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="13"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
@@ -781,7 +782,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
@@ -821,6 +822,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C8:C10"/>
@@ -828,11 +834,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -843,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F6A887-45A1-40AE-8AA4-AB98B07EB869}">
   <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,13 +856,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -872,101 +873,101 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="12">
         <v>0.99</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="12">
         <v>0.99</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="12">
         <v>0.8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="12">
         <v>0.97</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="12">
         <v>0.99</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="12">
         <v>0.8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="12">
         <v>0.9</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="12">
         <v>0.97</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="12">
         <v>0.9</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="14" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>